<commit_message>
Add orcad for crystal base
</commit_message>
<xml_diff>
--- a/Linhkien.xlsx
+++ b/Linhkien.xlsx
@@ -4,23 +4,25 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="18195" windowHeight="6465" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="18195" windowHeight="6465" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Attributes" sheetId="5" r:id="rId1"/>
     <sheet name="Màu" sheetId="1" r:id="rId2"/>
     <sheet name="IC" sheetId="2" r:id="rId3"/>
     <sheet name="Nguồn" sheetId="3" r:id="rId4"/>
-    <sheet name="Transitor" sheetId="4" r:id="rId5"/>
-    <sheet name="Jack" sheetId="6" r:id="rId6"/>
-    <sheet name="Led RGB" sheetId="7" r:id="rId7"/>
+    <sheet name="Transitor-C1815" sheetId="4" r:id="rId5"/>
+    <sheet name="Transitor-BC817" sheetId="8" r:id="rId6"/>
+    <sheet name="Jack" sheetId="6" r:id="rId7"/>
+    <sheet name="Led RGB" sheetId="7" r:id="rId8"/>
+    <sheet name="Dientro" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>GND</t>
   </si>
@@ -39,12 +41,45 @@
   <si>
     <t>0.24W</t>
   </si>
+  <si>
+    <t>Ic = 150mm</t>
+  </si>
+  <si>
+    <t>http://pdf1.alldatasheet.com/datasheet-pdf/view/16109/PHILIPS/BC817.html</t>
+  </si>
+  <si>
+    <t>http://glacier.lbl.gov/gtp/DSB/20040709_DSB_REVB.NET</t>
+  </si>
+  <si>
+    <t>http://www.hobby-hour.com/electronics/smdcalc.php</t>
+  </si>
+  <si>
+    <t>SMD</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R102   </t>
+  </si>
+  <si>
+    <t>SM/R_0603</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R103   </t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,8 +94,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -115,6 +172,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -125,10 +188,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -138,8 +202,14 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1106,6 +1176,66 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="8696325" cy="5219700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>276225</xdr:colOff>
       <xdr:row>2</xdr:row>
@@ -1249,7 +1379,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1898,20 +2028,50 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="G24"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A30"/>
+  <sheetViews>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A30" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1926,11 +2086,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
@@ -1939,4 +2099,72 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A1" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>